<commit_message>
Project Empty Project is saved.Test Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Empty Project/Main.xlsx
+++ b/DESIGN/rules/Empty Project/Main.xlsx
@@ -13,8 +13,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>Datatype aaa</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>aaaaaaa</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -29,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -37,12 +52,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,12 +378,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>